<commit_message>
added model classes for tables
</commit_message>
<xml_diff>
--- a/Documents/DB_plan.xlsx
+++ b/Documents/DB_plan.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TMohammad164855\Documents\Personal files\Work\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BB1A77-DB61-491D-8732-D9ED91F48C8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{6C413D68-4B18-4015-BFD4-C899A960FF06}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -149,8 +143,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,7 +242,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -300,7 +294,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -494,28 +488,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BB5A6F-9E5C-43EF-AAE6-C009AC672836}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="16.6328125" customWidth="1"/>
     <col min="4" max="4" width="64.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -526,7 +520,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -537,7 +531,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -548,7 +542,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -559,7 +553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -567,7 +561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -575,7 +569,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -586,7 +580,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -597,17 +591,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7">
       <c r="G9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7">
       <c r="G10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +612,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -629,7 +623,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -640,7 +634,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -651,7 +645,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -659,17 +653,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>20</v>
       </c>

</xml_diff>